<commit_message>
add new item to backup_list.xlsx
</commit_message>
<xml_diff>
--- a/backup_list.xlsx
+++ b/backup_list.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="企业内建安全工具" sheetId="1" r:id="rId1"/>
     <sheet name="扫描器" sheetId="2" r:id="rId2"/>
+    <sheet name="信息收集" sheetId="3" r:id="rId3"/>
+    <sheet name="弱口令生成" sheetId="4" r:id="rId4"/>
+    <sheet name="值得关注的github" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>巡风</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,6 +79,99 @@
   </si>
   <si>
     <t>F-NAScan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/Ekultek/Zeus-Scanner.git</t>
+  </si>
+  <si>
+    <t>Zeus-Scanner</t>
+  </si>
+  <si>
+    <t>http://www.freebuf.com/sectool/158355.html</t>
+  </si>
+  <si>
+    <t>taoman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>快速收集 https://src.edu-info.edu.cn 平台学校子域名工具</t>
+  </si>
+  <si>
+    <t>https://github.com/LandGrey/taoman.git</t>
+  </si>
+  <si>
+    <t>httpscan</t>
+  </si>
+  <si>
+    <t>轻量级信息收集工具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/5up3rc/httpscan.git</t>
+  </si>
+  <si>
+    <t>httpscan是一个扫描指定CIDR网段的Web主机的小工具。和端口扫描器不一样，httpscan是以爬虫的方式进行Web主机发现，因此相对来说不容易被防火墙拦截</t>
+  </si>
+  <si>
+    <t>genpAss</t>
+  </si>
+  <si>
+    <t>https://github.com/Tigascan/genpAss.git</t>
+  </si>
+  <si>
+    <t>中国特色的弱口令生成器</t>
+  </si>
+  <si>
+    <t>https://github.com/5up3rc</t>
+  </si>
+  <si>
+    <t>https://github.com/jas502n</t>
+  </si>
+  <si>
+    <t>https://github.com/RicterZ</t>
+  </si>
+  <si>
+    <t>https://github.com/alpha1e0/pentestdb.git</t>
+  </si>
+  <si>
+    <t>WEB渗透测试数据库</t>
+  </si>
+  <si>
+    <t>alpha1e0/pentestdb</t>
+  </si>
+  <si>
+    <t>资产验活工具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bitbucket.org/LaNMaSteR53/peepingtom.git</t>
+  </si>
+  <si>
+    <t>peepingtom</t>
+  </si>
+  <si>
+    <t>资产验活/自动截图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/ChrisTruncer/EyeWitness.git</t>
+  </si>
+  <si>
+    <t>EyeWitness</t>
+  </si>
+  <si>
+    <t>Github监控</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GSIL</t>
+  </si>
+  <si>
+    <t>https://github.com/FeeiCN/GSIL.git</t>
+  </si>
+  <si>
+    <t>实时监控Github敏感信息泄露，并发送告警通知</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -401,17 +497,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="47.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -447,6 +543,71 @@
       </c>
       <c r="B4" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -465,7 +626,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -515,5 +676,144 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="2" max="2" width="47.109375" customWidth="1"/>
+    <col min="3" max="3" width="54.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="57" customWidth="1"/>
+    <col min="3" max="3" width="43.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>